<commit_message>
Update the project issue tracking table
</commit_message>
<xml_diff>
--- a/project_issue_tracking_doc.xlsx
+++ b/project_issue_tracking_doc.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\src\Work Projects\carInfoSystem\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992CDF2B-9A9A-45A6-90B1-3647252DFD71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74A48A06-A2C6-4DAA-969B-F699B3E06C18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Описание</t>
   </si>
@@ -68,9 +62,6 @@
     <t>комуникация с други модули и интерфейс на приложението</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t xml:space="preserve">backend - connect db </t>
   </si>
   <si>
@@ -104,15 +95,6 @@
     <t>ui - vuejs</t>
   </si>
   <si>
-    <t>speedmeter</t>
-  </si>
-  <si>
-    <t>Радо, Данило</t>
-  </si>
-  <si>
-    <t xml:space="preserve">за момента готови </t>
-  </si>
-  <si>
     <t>документация</t>
   </si>
   <si>
@@ -122,13 +104,25 @@
     <t>Димитър</t>
   </si>
   <si>
-    <t>Трябва да се довършат още неща, 1-2 услуги в backend-a, визуалиция на данни във frontend.</t>
+    <t>speedmeter screen streeaming</t>
+  </si>
+  <si>
+    <t>screen streaming of the speedmeter app</t>
+  </si>
+  <si>
+    <t>screen streaming документация</t>
+  </si>
+  <si>
+    <t>документация относно screen streaming функционлаността</t>
+  </si>
+  <si>
+    <t>Радослав, Данило</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,9 +160,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -187,14 +182,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4D478E8-B309-4ABE-8556-D0543A3EF50B}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0">
-  <autoFilter ref="A1:E13" xr:uid="{4AD96A34-0828-4F75-BEDA-442D0D82708D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0">
+  <autoFilter ref="A1:E13"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C3E7B7E1-97B7-428F-BFF2-A4C85A3F7B71}" name="Задача"/>
-    <tableColumn id="2" xr3:uid="{C0674BC3-2CFF-40F8-B6A9-8A0500A378E9}" name="Описание"/>
-    <tableColumn id="3" xr3:uid="{00483C30-626E-4602-AB00-FF8AEEDB7608}" name="Възложена на"/>
-    <tableColumn id="4" xr3:uid="{CB6FF66E-44FD-4F5D-A6C8-6FDDFFCC660C}" name="Статус"/>
-    <tableColumn id="10" xr3:uid="{77B27258-46A2-4463-8BA2-2CE23A79F783}" name="Краен срок"/>
+    <tableColumn id="1" name="Задача"/>
+    <tableColumn id="2" name="Описание"/>
+    <tableColumn id="3" name="Възложена на"/>
+    <tableColumn id="4" name="Статус"/>
+    <tableColumn id="10" name="Краен срок"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -489,18 +484,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0330B74-30AF-4EDE-A760-B3F2FE42EB85}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,10 +557,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -576,10 +571,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -590,10 +585,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -604,10 +599,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -618,49 +613,58 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C11" t="s">
         <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>